<commit_message>
ASD en entities $2
</commit_message>
<xml_diff>
--- a/documents/gegevensanalyse ERD.xlsx
+++ b/documents/gegevensanalyse ERD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Educom\educom-VacIT\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D60E99A-3EB7-4FE3-BC4B-E960E3B66BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03758C1-629F-46FD-8750-EE6BA42279B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{38D5D0CB-C9D0-4FA3-89EF-EFE90E2C028B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{38D5D0CB-C9D0-4FA3-89EF-EFE90E2C028B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>naam</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>sollicitaties</t>
+  </si>
+  <si>
+    <t>compamy</t>
   </si>
 </sst>
 </file>
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A2997B-8869-4D48-B310-D7143B013A48}">
   <dimension ref="B1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +730,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
@@ -749,7 +752,7 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
@@ -767,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715494DC-C947-41EB-8FA6-B84E4AAF802A}">
   <dimension ref="B1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +883,7 @@
   <dimension ref="B1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>